<commit_message>
Added Amazon US links to the BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,29 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pro\Mobile-Robot-development-platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3921453-50ED-4E66-94AB-D1930B700288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEF38A7-1729-47F4-81BA-FBDF864C732C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>Average unit price</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Amazon UK</t>
   </si>
   <si>
@@ -40,134 +47,95 @@
     <t>Aliexpress</t>
   </si>
   <si>
-    <t xml:space="preserve">  bottom rod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Top Rod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  147 mm.step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  300 mm rod.step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  320 mm rod.step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  aluminum support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  aluminum support - 3</t>
-  </si>
-  <si>
-    <t>Base plate and body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Base Plate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Motor bracket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  planetary motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Pillow Block P08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  wheel axe</t>
-  </si>
-  <si>
     <t xml:space="preserve">  MD13S</t>
   </si>
   <si>
-    <t xml:space="preserve">  20mm spacer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  mid level plate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  82mm spacer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  RPLIDAR A1 DevKit.igs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  GT2_20Teeth_Pully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  70mm spacer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  motor support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Mecanum wheel 127mm L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Mecanum wheel 127mm R</t>
-  </si>
-  <si>
-    <t>Linear_actuator_2_inches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  linear_actuator_2inch_stroke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  shaft_2inches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  lifting mechanism - top plate</t>
-  </si>
-  <si>
-    <t>Lead acid battery place holder</t>
-  </si>
-  <si>
-    <t>side plates - 1</t>
-  </si>
-  <si>
-    <t>side plates</t>
-  </si>
-  <si>
-    <t>skin front top</t>
-  </si>
-  <si>
-    <t>skin front</t>
-  </si>
-  <si>
-    <t>skin front top slide</t>
-  </si>
-  <si>
-    <t>skin front side1</t>
-  </si>
-  <si>
-    <t>skin back side</t>
-  </si>
-  <si>
-    <t>skin Back</t>
-  </si>
-  <si>
-    <t>skin back top</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
     <t>No.</t>
   </si>
   <si>
-    <t>Cytron 13A motor Driver</t>
-  </si>
-  <si>
-    <t>8mm*</t>
+    <t>https://amzn.to/469Av5D</t>
+  </si>
+  <si>
+    <t>https://amzn.to/43MUS6W</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3JkuOYO</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3PjdtTO</t>
+  </si>
+  <si>
+    <t>Stainless steel  wheel axe</t>
+  </si>
+  <si>
+    <t>https://amzn.to/446CRjX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  100mm spacer</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3pcidA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RPLIDAR A1</t>
+  </si>
+  <si>
+    <t>https://amzn.to/4697vuS</t>
+  </si>
+  <si>
+    <t>https://amzn.to/4643zeK</t>
+  </si>
+  <si>
+    <t>24V Dc motor with planetary gearbox and bracket</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3CDJ4YM</t>
+  </si>
+  <si>
+    <t>Motor Encoder</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3pb6aTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mecanum wheel 127mm Left pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mecanum wheel 127mm Right pair</t>
+  </si>
+  <si>
+    <t>10pcs set of  Pillow Block P08</t>
+  </si>
+  <si>
+    <t>10pcs set of GT2 Pulley 20 Teeth 8mm Bore</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Amazon US Price</t>
+  </si>
+  <si>
+    <t>Amazon UK Price</t>
+  </si>
+  <si>
+    <t>Aliexpress Price</t>
+  </si>
+  <si>
+    <t>3D printed  motor support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,8 +270,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,8 +466,26 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -599,8 +600,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -643,14 +659,42 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -684,6 +728,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1004,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,449 +1061,377 @@
     <col min="2" max="2" width="46.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="1" customWidth="1"/>
-    <col min="5" max="8" width="9.140625" style="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="16.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="16.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D2" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2*C2</f>
+        <v>47.6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E12" si="0">D3*C3</f>
+        <v>139.19999999999999</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
+      <c r="D4" s="3">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.99</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>27.96</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>55.6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>99</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>9.99</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>9.99</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>9.67</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>38.68</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1">
         <v>1</v>
       </c>
+      <c r="D11" s="3">
+        <v>97.99</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>97.99</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>97.99</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>97.99</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
+      <c r="E15" s="1">
+        <f>SUM(E2:E12)</f>
+        <v>634</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(H2:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <f>SUM(K2:K12)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{95DFBB8B-4F45-46F7-BA94-733FF5054F4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the UK Amazon list
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pro\Mobile-Robot-development-platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEF38A7-1729-47F4-81BA-FBDF864C732C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8905CD0D-3495-435B-A4BC-C6C578B648C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="6585" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Item</t>
   </si>
@@ -129,6 +129,36 @@
   </si>
   <si>
     <t>3D printed  motor support</t>
+  </si>
+  <si>
+    <t>https://amzn.to/42Rv6xl</t>
+  </si>
+  <si>
+    <t>https://amzn.to/42Pd4eY</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3NFPgpq</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/uxcell-100mm-Stainless-Steel-Solid/dp/B082ZNFMXV?crid=1Q5VXEY9SXVP&amp;keywords=uxcell+8mm+x+100mm+304+Stainless+Steel+Solid+Round+Rod+for+DIY+Craft&amp;qid=1687284803&amp;sprefix=uxcell+8mm+x+100mm+304+stainless+steel+solid+round+rod+for+diy+craft%2Caps%2C113&amp;sr=8-2&amp;linkCode=sl1&amp;tag=mkeshk-21&amp;linkId=e972eecd57d27501cd172feb3130fbbc&amp;language=en_GB&amp;ref_=as_li_ss_tl</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3XjynnG</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3qL7LQm</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3pb38yN</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3qOruyJ</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3NkPTne</t>
+  </si>
+  <si>
+    <t>included in top link</t>
   </si>
 </sst>
 </file>
@@ -661,7 +691,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -691,6 +721,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1051,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1097,8 @@
     <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" style="1" customWidth="1"/>
     <col min="11" max="12" width="16.7109375" style="1" customWidth="1"/>
   </cols>
@@ -1094,7 +1128,7 @@
       <c r="H1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1124,12 +1158,19 @@
         <f>D2*C2</f>
         <v>47.6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="7">
+        <v>27.28</v>
+      </c>
+      <c r="H2" s="7">
+        <f>G2*C2</f>
+        <v>109.12</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -1151,12 +1192,19 @@
         <f t="shared" ref="E3:E12" si="0">D3*C3</f>
         <v>139.19999999999999</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="G3" s="7">
+        <v>28.08</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H12" si="1">G3*C3</f>
+        <v>112.32</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
@@ -1178,12 +1226,19 @@
         <f t="shared" si="0"/>
         <v>19.989999999999998</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="7">
+        <v>26.5</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
+        <v>26.5</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -1196,21 +1251,28 @@
         <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
         <v>6.99</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>27.96</v>
-      </c>
-      <c r="F5" s="4" t="s">
+        <v>13.98</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="G5" s="7">
+        <v>13.27</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="1"/>
+        <v>26.54</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -1235,9 +1297,16 @@
       <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1262,9 +1331,16 @@
       <c r="F7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="G7" s="7">
+        <v>99.9</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="1"/>
+        <v>99.9</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -1289,9 +1365,16 @@
       <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="G8" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
+        <v>7.8</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -1316,9 +1399,16 @@
       <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="7">
+        <v>16.62</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="1"/>
+        <v>66.48</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -1345,6 +1435,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="8"/>
@@ -1376,9 +1467,16 @@
       <c r="F11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="7">
+        <v>286.14999999999998</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="1"/>
+        <v>286.14999999999998</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -1404,8 +1502,13 @@
         <v>9</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
@@ -1416,11 +1519,11 @@
       </c>
       <c r="E15" s="1">
         <f>SUM(E2:E12)</f>
-        <v>634</v>
+        <v>620.02</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(H2:H12)</f>
-        <v>0</v>
+        <v>734.81</v>
       </c>
       <c r="K15" s="1">
         <f>SUM(K2:K12)</f>
@@ -1430,8 +1533,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1" xr:uid="{95DFBB8B-4F45-46F7-BA94-733FF5054F4D}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{1A130983-C69E-4030-8D88-D06B49F73BB3}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{1AB1A372-E249-4D7B-832D-BA7E26469B56}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{C1696A17-DDD5-4F59-BA26-932C770DA6AB}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{380DC7EE-76E6-4540-806C-B277DA6F1B74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Gt2 Belt to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pro\Mobile-Robot-development-platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537587AB-FE74-4B2B-A0B6-D1FE432E669B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF748BC5-601C-4623-9766-F77DC84FAB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/32566994011.html?spm=a2g0o.productlist.main.17.3f3c29884fD4j6&amp;algo_pvid=fb474dd6-0012-435e-9f79-31e775a1b10c&amp;algo_exp_id=fb474dd6-0012-435e-9f79-31e775a1b10c-8&amp;pdp_npi=3%40dis%21USD%219.08%217.17%21%21%21%21%21%40212278bd16874657618123638d07cd%2112000030636613730%21sea%21EG%21187121825&amp;curPageLogUid=4jLBiABnk315</t>
+  </si>
+  <si>
+    <t>Closed Gt2 Belt 6mm * 110mm</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3NMXYm9</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3CHSoLm</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_DEv5hNn</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1160,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J4" sqref="J4"/>
+      <selection pane="topRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1262,7 @@
         <v>34.799999999999997</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D12" si="0">C3*B3</f>
+        <f t="shared" ref="D3:D13" si="0">C3*B3</f>
         <v>139.19999999999999</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1260,7 +1272,7 @@
         <v>28.08</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G12" si="1">F3*B3</f>
+        <f t="shared" ref="G3:G13" si="1">F3*B3</f>
         <v>112.32</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1270,7 +1282,7 @@
         <v>341.98</v>
       </c>
       <c r="J3" s="15">
-        <f t="shared" ref="J3:J12" si="2">I3</f>
+        <f t="shared" ref="J3:J13" si="2">I3</f>
         <v>341.98</v>
       </c>
       <c r="K3" s="9" t="s">
@@ -1592,7 +1604,9 @@
       <c r="E12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
       <c r="G12" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1609,6 +1623,44 @@
       </c>
       <c r="K12" s="16" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>9.99</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>39.96</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="6">
+        <v>15.79</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="1"/>
+        <v>63.16</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.81</v>
+      </c>
+      <c r="J13" s="15">
+        <f t="shared" si="2"/>
+        <v>0.81</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -1629,16 +1681,16 @@
         <v>25</v>
       </c>
       <c r="D15" s="1">
-        <f>SUM(D2:D12)</f>
-        <v>620.02</v>
+        <f>SUM(D2:D13)</f>
+        <v>659.98</v>
       </c>
       <c r="G15" s="1">
-        <f>SUM(G2:G12)</f>
-        <v>734.81</v>
+        <f>SUM(G2:G13)</f>
+        <v>797.96999999999991</v>
       </c>
       <c r="J15" s="1">
-        <f>SUM(J2:J12)</f>
-        <v>467.7600000000001</v>
+        <f>SUM(J2:J13)</f>
+        <v>468.57000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>